<commit_message>
Avoid vector operation when value at pivot = 0
</commit_message>
<xml_diff>
--- a/explore/pseudoboolean/modular-operations-scaling.xlsx
+++ b/explore/pseudoboolean/modular-operations-scaling.xlsx
@@ -8,21 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryant/repos/pgbdd/explore/pseudoboolean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E739AAC-A040-EC40-B8C8-9EF58A7999E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479A9D12-9AC5-BC4A-A66C-044820013BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66720" yWindow="2800" windowWidth="35400" windowHeight="16440" xr2:uid="{544DE29A-88F0-0E4C-87E1-E71170600DAE}"/>
+    <workbookView xWindow="11340" yWindow="3920" windowWidth="28840" windowHeight="15860" xr2:uid="{544DE29A-88F0-0E4C-87E1-E71170600DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$4:$A$12</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$4:$A$13</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$4:$B$12</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$4:$C$13</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>N</t>
   </si>
@@ -52,21 +45,16 @@
     <t>Solving embedding of mutilated chessboard into modular arithmetic</t>
   </si>
   <si>
-    <t>Log N</t>
-  </si>
-  <si>
-    <t>Log Ops</t>
-  </si>
-  <si>
-    <t>N^3.9</t>
+    <t>N^C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -97,9 +85,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -266,43 +255,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5201</c:v>
+                  <c:v>1041</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11819</c:v>
+                  <c:v>1719</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23445</c:v>
+                  <c:v>2565</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42191</c:v>
+                  <c:v>3579</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70553</c:v>
+                  <c:v>4761</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>168029</c:v>
+                  <c:v>7629</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>343521</c:v>
+                  <c:v>11169</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>630821</c:v>
+                  <c:v>15381</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1069865</c:v>
+                  <c:v>20265</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2593649</c:v>
+                  <c:v>32049</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5357241</c:v>
+                  <c:v>46521</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9901313</c:v>
+                  <c:v>63681</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16864841</c:v>
+                  <c:v>83529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -435,43 +424,43 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2000</c:v>
+                  <c:v>1999.9999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4775.0623464010268</c:v>
+                  <c:v>3231.3687719817681</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9722.6780705212313</c:v>
+                  <c:v>4782.1831252056172</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17736.927283497822</c:v>
+                  <c:v>6661.343058260878</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29857.055729177879</c:v>
+                  <c:v>8876.5557765427657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>71284.651293397023</c:v>
+                  <c:v>14341.712569537318</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>145145.27049420375</c:v>
+                  <c:v>21224.657622264607</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>264786.21318388445</c:v>
+                  <c:v>29564.891601669326</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>445721.88840761589</c:v>
+                  <c:v>39396.621227037329</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1064174.9031509815</c:v>
+                  <c:v>63652.505777321181</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2166805.2149860151</c:v>
+                  <c:v>94200.928611027586</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3952868.3616746129</c:v>
+                  <c:v>131217.20466482939</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6653971.6309502712</c:v>
+                  <c:v>174853.15286456249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1574,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0C212E-D51D-A94F-B773-632AF2F4702F}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1585,20 +1574,20 @@
     <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>2000</v>
       </c>
-      <c r="C2" s="1">
-        <v>3.9</v>
+      <c r="C2" s="2">
+        <v>2.15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1606,265 +1595,163 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>5201</v>
+        <v>1041</v>
       </c>
       <c r="C4" s="1">
         <f>POWER(A4,$C$2)*B$2/POWER(A$4,$C$2)</f>
-        <v>2000</v>
-      </c>
-      <c r="E4">
-        <f>LOG(A4)</f>
-        <v>0.90308998699194354</v>
-      </c>
-      <c r="F4">
-        <f>LOG(B4)</f>
-        <v>3.7160868537748319</v>
+        <v>1999.9999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>11819</v>
+        <v>1719</v>
       </c>
       <c r="C5" s="1">
         <f>POWER(A5,$C$2)*B$2/POWER(A$4,$C$2)</f>
-        <v>4775.0623464010268</v>
+        <v>3231.3687719817681</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>12</v>
       </c>
       <c r="B6">
-        <v>23445</v>
+        <v>2565</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ref="C6:C16" si="0">POWER(A6,$C$2)*B$2/POWER(A$4,$C$2)</f>
-        <v>9722.6780705212313</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E16" si="1">LOG(A6)</f>
-        <v>1.0791812460476249</v>
-      </c>
-      <c r="F6">
-        <f t="shared" ref="F6:F16" si="2">LOG(B6)</f>
-        <v>4.3700502370748682</v>
+        <v>4782.1831252056172</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>42191</v>
+        <v>3579</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>17736.927283497822</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>1.146128035678238</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>4.625219819037607</v>
+        <v>6661.343058260878</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16</v>
       </c>
       <c r="B8">
-        <v>70553</v>
+        <v>4761</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>29857.055729177879</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>1.2041199826559248</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
-        <v>4.8485154852164509</v>
+        <v>8876.5557765427657</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20</v>
       </c>
       <c r="B9">
-        <v>168029</v>
+        <v>7629</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>71284.651293397023</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>1.3010299956639813</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>5.2253842427560508</v>
+        <v>14341.712569537318</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>24</v>
       </c>
       <c r="B10">
-        <v>343521</v>
+        <v>11169</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>145145.27049420375</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>1.3802112417116059</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>5.5359532913383598</v>
+        <v>21224.657622264607</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>28</v>
       </c>
       <c r="B11">
-        <v>630821</v>
+        <v>15381</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>264786.21318388445</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>1.4471580313422192</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>5.7999061425394158</v>
+        <v>29564.891601669326</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>32</v>
       </c>
       <c r="B12">
-        <v>1069865</v>
+        <v>20265</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>445721.88840761589</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>1.505149978319906</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>6.0293289800646734</v>
+        <v>39396.621227037329</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>40</v>
       </c>
       <c r="B13">
-        <v>2593649</v>
+        <v>32049</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>1064174.9031509815</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>1.6020599913279623</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
-        <v>6.4139112024044218</v>
+        <v>63652.505777321181</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>48</v>
       </c>
       <c r="B14">
-        <v>5357241</v>
+        <v>46521</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>2166805.2149860151</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>1.6812412373755872</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="2"/>
-        <v>6.7289411839154916</v>
+        <v>94200.928611027586</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>56</v>
       </c>
       <c r="B15">
-        <v>9901313</v>
+        <v>63681</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>3952868.3616746129</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>1.7481880270062005</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="2"/>
-        <v>6.9956927896323409</v>
+        <v>131217.20466482939</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>64</v>
       </c>
       <c r="B16">
-        <v>16864841</v>
+        <v>83529</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>6653971.6309502712</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>1.8061799739838871</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="2"/>
-        <v>7.2269822510604627</v>
+        <v>174853.15286456249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve performance through sparse-matrix data structures
</commit_message>
<xml_diff>
--- a/explore/pseudoboolean/modular-operations-scaling.xlsx
+++ b/explore/pseudoboolean/modular-operations-scaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryant/repos/pgbdd/explore/pseudoboolean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37F9024-384E-324C-8346-2A1985331D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC68C8DC-30B9-E046-9AD5-24FA24A5B147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11340" yWindow="3920" windowWidth="28840" windowHeight="15860" xr2:uid="{544DE29A-88F0-0E4C-87E1-E71170600DAE}"/>
   </bookViews>
@@ -202,10 +202,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$16</c:f>
+              <c:f>Sheet1!$A$4:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -244,16 +244,28 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$16</c:f>
+              <c:f>Sheet1!$B$4:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1041</c:v>
                 </c:pt>
@@ -292,6 +304,18 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>83529</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131289</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>189801</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>259065</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>339081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -371,10 +395,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$16</c:f>
+              <c:f>Sheet1!$A$4:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -413,54 +437,78 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$16</c:f>
+              <c:f>Sheet1!$C$4:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1999.9999999999998</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3231.3687719817681</c:v>
+                  <c:v>3181.2867944764967</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4782.1831252056172</c:v>
+                  <c:v>4648.3606331383126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6661.343058260878</c:v>
+                  <c:v>6405.4424990535663</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8876.5557765427657</c:v>
+                  <c:v>8456.1443244910461</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14341.712569537318</c:v>
+                  <c:v>13450.710135845362</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21224.657622264607</c:v>
+                  <c:v>19653.604193050076</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29564.891601669326</c:v>
+                  <c:v>27082.673117112783</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39396.621227037329</c:v>
+                  <c:v>35753.188418311038</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63652.505777321181</c:v>
+                  <c:v>56870.573087801429</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>94200.928611027586</c:v>
+                  <c:v>83096.856776426852</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>131217.20466482939</c:v>
+                  <c:v>114507.49628565976</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>174853.15286456249</c:v>
+                  <c:v>151167.06066297984</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>240452.8869234825</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>351339.50690651371</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>484145.95741382992</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>639145.24103762547</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -488,7 +536,7 @@
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="64"/>
+          <c:max val="128"/>
           <c:min val="8"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -553,7 +601,7 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="100000000"/>
+          <c:max val="1000000"/>
           <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1563,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0C212E-D51D-A94F-B773-632AF2F4702F}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1584,7 +1632,7 @@
         <v>2000</v>
       </c>
       <c r="C2" s="2">
-        <v>2.15</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1607,7 +1655,7 @@
       </c>
       <c r="C4" s="1">
         <f>POWER(A4,$C$2)*B$2/POWER(A$4,$C$2)</f>
-        <v>1999.9999999999998</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1619,7 +1667,7 @@
       </c>
       <c r="C5" s="1">
         <f>POWER(A5,$C$2)*B$2/POWER(A$4,$C$2)</f>
-        <v>3231.3687719817681</v>
+        <v>3181.2867944764967</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1630,8 +1678,8 @@
         <v>2565</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:C16" si="0">POWER(A6,$C$2)*B$2/POWER(A$4,$C$2)</f>
-        <v>4782.1831252056172</v>
+        <f t="shared" ref="C6:C20" si="0">POWER(A6,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>4648.3606331383126</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1643,7 +1691,7 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>6661.343058260878</v>
+        <v>6405.4424990535663</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1655,7 +1703,7 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>8876.5557765427657</v>
+        <v>8456.1443244910461</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1667,7 +1715,7 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>14341.712569537318</v>
+        <v>13450.710135845362</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1679,7 +1727,7 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>21224.657622264607</v>
+        <v>19653.604193050076</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1691,7 +1739,7 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>29564.891601669326</v>
+        <v>27082.673117112783</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1703,7 +1751,7 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>39396.621227037329</v>
+        <v>35753.188418311038</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1715,7 +1763,7 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>63652.505777321181</v>
+        <v>56870.573087801429</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1727,7 +1775,7 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>94200.928611027586</v>
+        <v>83096.856776426852</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1739,7 +1787,7 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>131217.20466482939</v>
+        <v>114507.49628565976</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1751,7 +1799,55 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>174853.15286456249</v>
+        <v>151167.06066297984</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>131289</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>240452.8869234825</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>96</v>
+      </c>
+      <c r="B18">
+        <v>189801</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>351339.50690651371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>259065</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>484145.95741382992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>128</v>
+      </c>
+      <c r="B20">
+        <v>339081</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>639145.24103762547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed for even modulus
</commit_message>
<xml_diff>
--- a/explore/pseudoboolean/modular-operations-scaling.xlsx
+++ b/explore/pseudoboolean/modular-operations-scaling.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryant/repos/pgbdd/explore/pseudoboolean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC68C8DC-30B9-E046-9AD5-24FA24A5B147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93062862-CDD6-014B-AC77-81F54AECD34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="3920" windowWidth="28840" windowHeight="15860" xr2:uid="{544DE29A-88F0-0E4C-87E1-E71170600DAE}"/>
+    <workbookView xWindow="7620" yWindow="1220" windowWidth="28840" windowHeight="15860" activeTab="2" xr2:uid="{544DE29A-88F0-0E4C-87E1-E71170600DAE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MCB Operations" sheetId="1" r:id="rId1"/>
+    <sheet name="MCB Nonzeros" sheetId="2" r:id="rId2"/>
+    <sheet name="MCB Nonzeros Randomized" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>N</t>
   </si>
@@ -46,6 +48,9 @@
   </si>
   <si>
     <t>N^C</t>
+  </si>
+  <si>
+    <t>Nonzeros</t>
   </si>
 </sst>
 </file>
@@ -131,7 +136,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$3</c:f>
+              <c:f>'MCB Operations'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -202,7 +207,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$20</c:f>
+              <c:f>'MCB Operations'!$A$4:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -262,7 +267,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$20</c:f>
+              <c:f>'MCB Operations'!$B$4:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -395,7 +400,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$20</c:f>
+              <c:f>'MCB Operations'!$A$4:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -455,7 +460,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$20</c:f>
+              <c:f>'MCB Operations'!$C$4:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -731,7 +736,1337 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MCB Nonzeros'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nonzeros</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros'!$B$4:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4709</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15317</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24029</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35525</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>68405</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>117029</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>184469</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>273797</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>530405</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>911429</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1441445</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2145029</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DF36-9547-93A3-2DD22ADE4DD8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trend</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros'!$C$4:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1953.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5359.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>216000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>343000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>512000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1728000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2744000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4096000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DF36-9547-93A3-2DD22ADE4DD8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1388773584"/>
+        <c:axId val="1389361440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1388773584"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:max val="128"/>
+          <c:min val="8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1389361440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1389361440"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="10000000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1388773584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MCB Nonzeros Randomized'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nonzeros</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros Randomized'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros Randomized'!$B$4:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>646</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1471</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2410</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4229</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17059</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19472</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32752</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66016</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>117029</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>192822</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>344385</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>723815</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1524484</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2455532</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4941507</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-88E7-084E-A5B5-17FCC5E7523F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trend</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros Randomized'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros Randomized'!$C$4:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2042.2647511548332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3660.0922277922346</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5994.0692460782757</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9189.5868399762749</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18767.569280959862</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33634.735369619018</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55083.019861667482</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84448.506289465353</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>172466.20768265193</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>309089.32151873579</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>506190.19442693266</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>776046.88205332379</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1584893.1924611116</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2840403.1614057673</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4651678.7492307592</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7131550.2145218495</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-88E7-084E-A5B5-17FCC5E7523F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1388773584"/>
+        <c:axId val="1389361440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1388773584"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:max val="128"/>
+          <c:min val="8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1389361440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1389361440"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="10000000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1388773584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1273,6 +2608,1010 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1298,6 +3637,92 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292485</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>116481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333536</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>192424</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00D41722-69AE-7547-A859-3F9CF5E73736}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292485</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>116481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333536</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>192424</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CC9F297-706E-4D43-A6F9-7C2FA92ADC72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1613,8 +4038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0C212E-D51D-A94F-B773-632AF2F4702F}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1854,4 +4279,498 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2692AD-81BD-BD4C-97F7-A26C56EE35E6}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>629</v>
+      </c>
+      <c r="C4" s="1">
+        <f>POWER(A4,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1205</v>
+      </c>
+      <c r="C5" s="1">
+        <f>POWER(A5,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>1953.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>2045</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:C20" si="0">POWER(A6,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>3197</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>5359.375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>4709</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>9005</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>15625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>15317</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>24029</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>42875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>35525</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>64000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>68405</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>117029</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>216000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>184469</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>343000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>273797</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>512000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>530405</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>96</v>
+      </c>
+      <c r="B18">
+        <v>911429</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>1728000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>1441445</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>2744000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>128</v>
+      </c>
+      <c r="B20">
+        <v>2145029</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>4096000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB198C8-CD29-6043-8A37-F3953E64CD91}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>646</v>
+      </c>
+      <c r="C4" s="1">
+        <f>POWER(A4,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1471</v>
+      </c>
+      <c r="C5" s="1">
+        <f>POWER(A5,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>2042.2647511548332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>2410</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:C20" si="0">POWER(A6,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>3660.0922277922346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>3300</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>5994.0692460782757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>4229</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>9189.5868399762749</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>7652</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>18767.569280959862</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>17059</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>33634.735369619018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>19472</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>55083.019861667482</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>32752</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>84448.506289465353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>66016</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>172466.20768265193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>117029</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>309089.32151873579</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>192822</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>506190.19442693266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>344385</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>776046.88205332379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>723815</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>1584893.1924611116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>96</v>
+      </c>
+      <c r="B18">
+        <v>1524484</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>2840403.1614057673</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>2455532</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>4651678.7492307592</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>128</v>
+      </c>
+      <c r="B20">
+        <v>4941507</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>7131550.2145218495</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add estimates of BDD operations
</commit_message>
<xml_diff>
--- a/explore/pseudoboolean/modular-operations-scaling.xlsx
+++ b/explore/pseudoboolean/modular-operations-scaling.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryant/repos/pgbdd/explore/pseudoboolean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93062862-CDD6-014B-AC77-81F54AECD34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F20338E-59A2-8C4C-A6B8-9EEDB771CC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="1220" windowWidth="28840" windowHeight="15860" activeTab="2" xr2:uid="{544DE29A-88F0-0E4C-87E1-E71170600DAE}"/>
+    <workbookView xWindow="5320" yWindow="5640" windowWidth="28840" windowHeight="15860" firstSheet="1" activeTab="5" xr2:uid="{544DE29A-88F0-0E4C-87E1-E71170600DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="MCB Operations" sheetId="1" r:id="rId1"/>
-    <sheet name="MCB Nonzeros" sheetId="2" r:id="rId2"/>
-    <sheet name="MCB Nonzeros Randomized" sheetId="3" r:id="rId3"/>
+    <sheet name="MCB Operations Randomized" sheetId="4" r:id="rId2"/>
+    <sheet name="MCB Nonzeros" sheetId="2" r:id="rId3"/>
+    <sheet name="MCB Nonzeros Randomized" sheetId="3" r:id="rId4"/>
+    <sheet name="MCB Nonzeros Rand MinFill" sheetId="5" r:id="rId5"/>
+    <sheet name="MCB BDD Ops Rand MinFill" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>N</t>
   </si>
@@ -51,6 +54,9 @@
   </si>
   <si>
     <t>Nonzeros</t>
+  </si>
+  <si>
+    <t>Poly Trend</t>
   </si>
 </sst>
 </file>
@@ -761,6 +767,631 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>'MCB Operations Randomized'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Operations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB Operations Randomized'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB Operations Randomized'!$B$4:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1329</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2064</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2886</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3903</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9444</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17364</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40530</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57081</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>74292</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>118800</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>171348</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>235482</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>312729</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EEE9-8C48-9253-50954D185176}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trend</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB Operations Randomized'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB Operations Randomized'!$C$4:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>809.64685349684316</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1200.4031430950013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1674.6813717829243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2234.5742761444403</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3618.4320631706601</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5364.779969126047</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7484.399828248811</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9986.6443912128962</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16171.310416674836</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23975.998632368057</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33448.894657169381</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44631.797323212981</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72271.988537296362</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>107152.29957752774</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>149488.07913275136</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>199466.13239308813</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EEE9-8C48-9253-50954D185176}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1388773584"/>
+        <c:axId val="1389361440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1388773584"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:max val="128"/>
+          <c:min val="8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1389361440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1389361440"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1000000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1388773584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'MCB Nonzeros'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1361,7 +1992,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1772,6 +2403,1256 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-88E7-084E-A5B5-17FCC5E7523F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1388773584"/>
+        <c:axId val="1389361440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1388773584"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:max val="128"/>
+          <c:min val="8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1389361440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1389361440"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="10000000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1388773584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MCB Nonzeros Rand MinFill'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nonzeros</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros Rand MinFill'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros Rand MinFill'!$B$4:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1244</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2561</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4304</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8819</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11909</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19735</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29229</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39484</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52844</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>83986</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>123338</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>169193</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>223294</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9A95-0D40-A1F1-7AB5F70B2EC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trend</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros Rand MinFill'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB Nonzeros Rand MinFill'!$C$4:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1652.1425991258839</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2490.0343193257263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3522.3751579927853</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4756.8284600108873</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7858.958935518348</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11844.666116572442</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16755.334398375413</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22627.416997969529</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>37383.719530530521</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56343.044882638431</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>79702.251523191619</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>107634.74115247537</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>177827.94100389211</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>268014.19942140474</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>379129.93837246334</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>511999.99999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9A95-0D40-A1F1-7AB5F70B2EC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1388773584"/>
+        <c:axId val="1389361440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1388773584"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:max val="128"/>
+          <c:min val="8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1389361440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1389361440"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="10000000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1388773584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MCB BDD Ops Rand MinFill'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nonzeros</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB BDD Ops Rand MinFill'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB BDD Ops Rand MinFill'!$B$4:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>4914</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13383</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20475</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26946</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45126</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63639</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92241</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>204687</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>302499</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>408789</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>546480</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>867591</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1271511</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1743048</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2299077</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1697-B94E-BB36-BE4A1575745B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trend</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MCB BDD Ops Rand MinFill'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MCB BDD Ops Rand MinFill'!$C$4:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16374.616172486574</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24499.75167813744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34444.040213304288</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46267.527356211518</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75761.300170798539</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>113354.29309886131</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>159364.05728275061</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>214068.40876577795</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>350528.80281945708</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>524462.28568955802</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>737338.08799265279</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>990441.59586712916</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1621810.097358929</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2426557.3150442825</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3411481.0156976678</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4582528.3631512159</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1697-B94E-BB36-BE4A1575745B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2106,6 +3987,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
   <cs:axisTitle>
@@ -3111,6 +5112,1512 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3673,7 +7180,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00D41722-69AE-7547-A859-3F9CF5E73736}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83980B96-09DE-BD4D-B65D-47EDE8F53DCE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3716,7 +7223,136 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00D41722-69AE-7547-A859-3F9CF5E73736}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292485</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>116481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333536</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>192424</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CC9F297-706E-4D43-A6F9-7C2FA92ADC72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292485</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>116481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333536</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>192424</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1B5B54A-2B5C-8247-B892-26202910679A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292485</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>116481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333536</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>192424</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E33133D-E65F-B94E-B20D-52BBA6D1232E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4282,6 +7918,253 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F80DBE1-5AE4-1D4B-8EAD-40DA511CB3C9}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>810</v>
+      </c>
+      <c r="C4" s="1">
+        <f>POWER(A4,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1329</v>
+      </c>
+      <c r="C5" s="1">
+        <f>POWER(A5,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>809.64685349684316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>2064</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:C20" si="0">POWER(A6,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>1200.4031430950013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>2886</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>1674.6813717829243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>3903</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>2234.5742761444403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>6432</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>3618.4320631706601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>9444</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>5364.779969126047</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>12993</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>7484.399828248811</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>17364</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>9986.6443912128962</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>28005</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>16171.310416674836</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>40530</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>23975.998632368057</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>57081</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>33448.894657169381</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>74292</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>44631.797323212981</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>118800</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>72271.988537296362</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>96</v>
+      </c>
+      <c r="B18">
+        <v>171348</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>107152.29957752774</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>235482</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>149488.07913275136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>128</v>
+      </c>
+      <c r="B20">
+        <v>312729</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>199466.13239308813</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2692AD-81BD-BD4C-97F7-A26C56EE35E6}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -4528,12 +8411,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB198C8-CD29-6043-8A37-F3953E64CD91}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4773,4 +8656,498 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1562572E-8866-094A-AE2A-238D1EA058C3}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>448</v>
+      </c>
+      <c r="C4" s="1">
+        <f>POWER(A4,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>748</v>
+      </c>
+      <c r="C5" s="1">
+        <f>POWER(A5,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>1652.1425991258839</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1244</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:C20" si="0">POWER(A6,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>2490.0343193257263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>1941</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>3522.3751579927853</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>2561</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>4756.8284600108873</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>4304</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>7858.958935518348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>6019</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>11844.666116572442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>8819</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>16755.334398375413</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>11909</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>22627.416997969529</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>19735</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>37383.719530530521</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>29229</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>56343.044882638431</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>39484</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>79702.251523191619</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>52844</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>107634.74115247537</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>83986</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>177827.94100389211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>96</v>
+      </c>
+      <c r="B18">
+        <v>123338</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>268014.19942140474</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>169193</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>379129.93837246334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>128</v>
+      </c>
+      <c r="B20">
+        <v>223294</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>511999.99999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D964F376-F3DA-ED49-B650-60DA3AFC5D76}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>10000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>4914</v>
+      </c>
+      <c r="C4" s="1">
+        <f>POWER(A4,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>8199</v>
+      </c>
+      <c r="C5" s="1">
+        <f>POWER(A5,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>16374.616172486574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>13383</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:C20" si="0">POWER(A6,$C$2)*B$2/POWER(A$4,$C$2)</f>
+        <v>24499.75167813744</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>20475</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>34444.040213304288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>26946</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>46267.527356211518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>45126</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>75761.300170798539</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>63639</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>113354.29309886131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>92241</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>159364.05728275061</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>124281</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>214068.40876577795</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>204687</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>350528.80281945708</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <v>302499</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>524462.28568955802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>408789</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>737338.08799265279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>546480</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>990441.59586712916</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>867591</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>1621810.097358929</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>96</v>
+      </c>
+      <c r="B18">
+        <v>1271511</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>2426557.3150442825</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>112</v>
+      </c>
+      <c r="B19">
+        <v>1743048</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>3411481.0156976678</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>128</v>
+      </c>
+      <c r="B20">
+        <v>2299077</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>4582528.3631512159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>